<commit_message>
[Farm] 작물 수확시 Farmer FarmingSkill 스탯 적용
</commit_message>
<xml_diff>
--- a/DataTable/FarmerConfigTable.xlsx
+++ b/DataTable/FarmerConfigTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\ProjectF\DataTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seh00n/GitHub/ProjectF/DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2AD3E53-BBCC-49C5-B688-E7A2C1ACD9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938EFE8F-920B-A54C-9E09-7417B04EB4CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FA5AC356-2F7D-4E04-A31B-16325DD2973F}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="29040" windowHeight="15720" xr2:uid="{FA5AC356-2F7D-4E04-A31B-16325DD2973F}"/>
   </bookViews>
   <sheets>
     <sheet name="FarmerConfigTable" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>id</t>
   </si>
@@ -77,6 +77,10 @@
   </si>
   <si>
     <t>Base=ConfigTable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FarmingSkillFactor</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -84,7 +88,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,7 +148,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -155,6 +159,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -491,26 +501,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBA55706-2B54-42AF-9FA4-0B5212D393DB}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="13.875" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
     <col min="2" max="2" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="25.125" customWidth="1"/>
-    <col min="4" max="4" width="17.125" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -521,7 +531,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -532,7 +542,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -543,7 +553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -554,7 +564,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -565,7 +575,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -574,6 +584,17 @@
       </c>
       <c r="C7" s="3">
         <v>1.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="4">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>